<commit_message>
minor change to age similarity matrix
</commit_message>
<xml_diff>
--- a/Data/similarityAge_TAX.xlsx
+++ b/Data/similarityAge_TAX.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Castaire\Desktop\analysis_attempt\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Castaire\Desktop\kizune\STAT450-550-Project-GovtAgencies\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F05BF7E2-A384-49CF-A1F0-D235D3F2F6AD}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9BC00E0-D169-4FAE-964A-F3CA5F9E3498}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6940" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -466,8 +466,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AF33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="U9" sqref="U9"/>
+    <sheetView tabSelected="1" topLeftCell="W1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A26" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I6" sqref="I6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>